<commit_message>
did some worrk on files
done some writing lm,fao
</commit_message>
<xml_diff>
--- a/asset list.xlsx
+++ b/asset list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c0999686\Documents\GitHub\Gnomes-on-the-roam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal Projects\Gnomes-on-the-roam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717FD23-27DA-4931-9D45-E675620B0E77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BF963-BE33-417F-B900-137711FA0D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A025463A-1597-42AE-AF35-739BFE196A9F}"/>
+    <workbookView xWindow="5850" yWindow="5850" windowWidth="43200" windowHeight="23985" xr2:uid="{A025463A-1597-42AE-AF35-739BFE196A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>2 hours</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>Fly_trap_v03</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve">buyable door </t>
+  </si>
+  <si>
+    <t>6h</t>
   </si>
 </sst>
 </file>
@@ -293,12 +293,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -618,7 +617,7 @@
   <dimension ref="B4:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +811,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
@@ -820,10 +819,10 @@
       <c r="K11" s="2"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="O11" s="1"/>
     </row>
@@ -1237,15 +1236,15 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="4" t="s">
-        <v>56</v>
+      <c r="C31" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="4" t="s">
-        <v>60</v>
+      <c r="F31" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="2"/>
@@ -1259,15 +1258,15 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="4" t="s">
-        <v>57</v>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="4" t="s">
-        <v>61</v>
+      <c r="F32" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="2"/>
@@ -1281,15 +1280,15 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
-      <c r="C33" s="4" t="s">
-        <v>58</v>
+      <c r="C33" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="4" t="s">
-        <v>62</v>
+      <c r="F33" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="2"/>
@@ -1303,15 +1302,15 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
-      <c r="C34" s="4" t="s">
-        <v>59</v>
+      <c r="C34" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="4" t="s">
-        <v>63</v>
+      <c r="F34" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>

</xml_diff>